<commit_message>
Update study results with Usha and Phoebe data
</commit_message>
<xml_diff>
--- a/study/data/stats/combined/stats-combined-eval-diff.xlsx
+++ b/study/data/stats/combined/stats-combined-eval-diff.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1716" windowWidth="39864" windowHeight="19488"/>
+    <workbookView xWindow="1176" yWindow="6768" windowWidth="39864" windowHeight="10548"/>
   </bookViews>
   <sheets>
     <sheet name="Eval Difference" sheetId="17" r:id="rId1"/>
@@ -31,9 +31,9 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Eval Difference'!$A$1:$AF$33</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">src_adam!$A$1:$AB$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">src_kenton!$A$1:$AB$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">src_phoebe!$A$1:$AB$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">src_phoebe!$A$1:$AB$33</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">src_susan!$A$1:$AB$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">src_usha!$A$1:$AB$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">src_usha!$A$1:$AB$32</definedName>
     <definedName name="SUSAN_ALL">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -528,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -703,6 +703,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,8 +748,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.1479369833252499E-2"/>
-          <c:y val="4.866868493290194E-2"/>
+          <c:x val="5.1479369833252492E-2"/>
+          <c:y val="4.8668684932901961E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -760,6 +763,77 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:spPr/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:spPr/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.5261738360866663E-17"/>
+                  <c:y val="1.4584411406833472E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1100" b="1">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showVal val="1"/>
+            </c:dLbl>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -861,22 +935,22 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.57820655413541455</c:v>
+                  <c:v>0.49206401474889361</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42144172856989848</c:v>
+                  <c:v>0.36683949537962146</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75061061263786188</c:v>
+                  <c:v>0.66741306690111002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41301453889048145</c:v>
+                  <c:v>0.37450246124465336</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.50597538917196072</c:v>
+                  <c:v>0.39585999526617538</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8.831683168316834E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.21264298615291993</c:v>
@@ -888,7 +962,7 @@
                   <c:v>0.59918157486970003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>8.8888888888888892E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.1074087903805967</c:v>
@@ -903,13 +977,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1.8316831683168319E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>0.15831683168316829</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>6.1485148514851491E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.6037704523580365</c:v>
@@ -930,7 +1004,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.5501370713927175</c:v>
+                  <c:v>0.46077175864775277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -938,11 +1012,11 @@
         </c:ser>
         <c:gapWidth val="55"/>
         <c:overlap val="-7"/>
-        <c:axId val="51530368"/>
-        <c:axId val="51544448"/>
+        <c:axId val="35342592"/>
+        <c:axId val="46956544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51530368"/>
+        <c:axId val="35342592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -961,14 +1035,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51544448"/>
+        <c:crossAx val="46956544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51544448"/>
+        <c:axId val="46956544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -976,7 +1050,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51530368"/>
+        <c:crossAx val="35342592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -986,7 +1060,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1024,8 +1098,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.48032248449649434"/>
-          <c:y val="0.14860989598522412"/>
+          <c:x val="0.4803224844964944"/>
+          <c:y val="0.14860989598522417"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1043,8 +1117,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.446897417866869E-7"/>
-                  <c:y val="5.9846685830937853E-3"/>
+                  <c:x val="-1.4468974178668682E-7"/>
+                  <c:y val="1.2146021026484443E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr/>
@@ -1055,7 +1129,10 @@
                   <a:pPr>
                     <a:defRPr sz="1100" b="1">
                       <a:solidFill>
-                        <a:schemeClr val="tx1"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
                       </a:solidFill>
                     </a:defRPr>
                   </a:pPr>
@@ -1070,7 +1147,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0"/>
-                  <c:y val="1.5026825350534892E-2"/>
+                  <c:y val="8.8654237074339837E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr/>
@@ -1081,7 +1158,10 @@
                   <a:pPr>
                     <a:defRPr sz="1100" b="1">
                       <a:solidFill>
-                        <a:schemeClr val="tx1"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
                       </a:solidFill>
                     </a:defRPr>
                   </a:pPr>
@@ -1096,7 +1176,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0"/>
-                  <c:y val="6.730478134677613E-2"/>
+                  <c:y val="6.7304781346776144E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr/>
@@ -1107,7 +1187,10 @@
                   <a:pPr>
                     <a:defRPr sz="1100" b="1">
                       <a:solidFill>
-                        <a:schemeClr val="tx1"/>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
                       </a:solidFill>
                     </a:defRPr>
                   </a:pPr>
@@ -1182,13 +1265,13 @@
                   <c:v>8.4180225281601989E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.6631716906946274E-2</c:v>
+                  <c:v>7.9385826771653553E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.3794037940379409E-3</c:v>
+                  <c:v>-8.7523277467411586E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5501370713927175</c:v>
+                  <c:v>0.46077175864775277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1196,11 +1279,11 @@
         </c:ser>
         <c:gapWidth val="55"/>
         <c:overlap val="-7"/>
-        <c:axId val="51567232"/>
-        <c:axId val="51712384"/>
+        <c:axId val="67275776"/>
+        <c:axId val="67416832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51567232"/>
+        <c:axId val="67275776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1222,14 +1305,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51712384"/>
+        <c:crossAx val="67416832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51712384"/>
+        <c:axId val="67416832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1238,7 +1321,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51567232"/>
+        <c:crossAx val="67275776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1248,7 +1331,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1610,7 +1693,7 @@
   <dimension ref="A1:AL32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC50" sqref="AC50"/>
+      <selection activeCell="AU17" sqref="AU17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1936,36 +2019,36 @@
       </c>
       <c r="T7" s="27">
         <f>IF(V7="", "", (src_susan!S10*src_susan!U10 + src_adam!S10*src_adam!U10 + src_kenton!S10*src_kenton!U10 + src_phoebe!S10*src_phoebe!U10 + src_usha!S10*src_usha!U10)/V7)</f>
-        <v>0.15528089887640451</v>
+        <v>0.12388157894736844</v>
       </c>
       <c r="U7" s="27">
         <f>IF(V7="", "", SQRT((IF(src_susan!U10&gt;1, (src_susan!U10-1)*(src_susan!T10^2), 0) + IF(src_adam!U10&gt;1, (src_adam!U10-1)*(src_adam!T10^2), 0) + IF(src_kenton!U10&gt;1, (src_kenton!U10-1)*(src_kenton!T10^2), 0) + IF(src_phoebe!U10&gt;1, (src_phoebe!U10-1)*(src_phoebe!T10^2), 0) + IF(src_usha!U10&gt;1, (src_usha!U10-1)*(src_usha!T10^2), 0)) / (V7 - COUNTIF(V7:V7, ""))))</f>
-        <v>0.93386775764240038</v>
+        <v>0.84311179567125016</v>
       </c>
       <c r="V7" s="9">
         <f>IF((src_susan!U10 + src_adam!U10 + src_kenton!U10 + src_phoebe!U10 + src_usha!U10)=0, "", (src_susan!U10 + src_adam!U10 + src_kenton!U10 + src_phoebe!U10 + src_usha!U10))</f>
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="X7" s="27">
         <f>IF(Z7="", "", (src_susan!W10*src_susan!Y10 + src_adam!W10*src_adam!Y10 + src_kenton!W10*src_kenton!Y10 + src_phoebe!W10*src_phoebe!Y10 + src_usha!W10*src_usha!Y10)/Z7)</f>
-        <v>0.13936507936507936</v>
+        <v>0.11544117647058823</v>
       </c>
       <c r="Y7" s="27">
         <f>IF(Z7="", "", SQRT((IF(src_susan!Y10&gt;1, (src_susan!Y10-1)*(src_susan!X10^2), 0) + IF(src_adam!Y10&gt;1, (src_adam!Y10-1)*(src_adam!X10^2), 0) + IF(src_kenton!Y10&gt;1, (src_kenton!Y10-1)*(src_kenton!X10^2), 0) + IF(src_phoebe!Y10&gt;1, (src_phoebe!Y10-1)*(src_phoebe!X10^2), 0) + IF(src_usha!Y10&gt;1, (src_usha!Y10-1)*(src_usha!X10^2), 0)) / (Z7 - COUNTIF(Z7:Z7, ""))))</f>
-        <v>0.57488853301907616</v>
+        <v>0.54710199070675491</v>
       </c>
       <c r="Z7" s="9">
         <f>IF((src_susan!Y10 + src_adam!Y10 + src_kenton!Y10 + src_phoebe!Y10 + src_usha!Y10)=0, "", (src_susan!Y10 + src_adam!Y10 + src_kenton!Y10 + src_phoebe!Y10 + src_usha!Y10))</f>
-        <v>189</v>
+        <v>272</v>
       </c>
       <c r="AA7" s="9"/>
       <c r="AB7" s="28">
         <f>IF(F7="", "", (D7*H7 + H7*J7 + L7*N7 + P7*R7 + T7*V7 + X7*Z7) / (H7 + J7 + N7 + R7 + V7 + Z7))</f>
-        <v>0.57820655413541455</v>
+        <v>0.49206401474889361</v>
       </c>
       <c r="AC7" s="52">
         <f>AB7-AVG_ALL</f>
-        <v>2.8069482742697049E-2</v>
+        <v>3.1292256101140836E-2</v>
       </c>
       <c r="AD7" s="28">
         <f>IF(SUM(F7, J7, N7, R7, V7, Z7)&lt;=1, "", SQRT(
@@ -1977,7 +2060,7 @@
    IF(Z7&gt;1, (Z7-1)*Y7^2, 0)) /
   (SUM(F7, J7, N7, R7, V7, Z7) - 6)
 ))</f>
-        <v>1.2234409894119809</v>
+        <v>1.1500528987808367</v>
       </c>
       <c r="AE7" s="8"/>
       <c r="AF7" s="18" t="s">
@@ -2041,36 +2124,36 @@
       </c>
       <c r="T8" s="27">
         <f>IF(V8="", "", (src_susan!S11*src_susan!U11 + src_adam!S11*src_adam!U11 + src_kenton!S11*src_kenton!U11 + src_phoebe!S11*src_phoebe!U11 + src_usha!S11*src_usha!U11)/V8)</f>
-        <v>0.10000000000000002</v>
+        <v>0.13640522875816993</v>
       </c>
       <c r="U8" s="27">
         <f>IF(V8="", "", SQRT((IF(src_susan!U11&gt;1, (src_susan!U11-1)*(src_susan!T11^2), 0) + IF(src_adam!U11&gt;1, (src_adam!U11-1)*(src_adam!T11^2), 0) + IF(src_kenton!U11&gt;1, (src_kenton!U11-1)*(src_kenton!T11^2), 0) + IF(src_phoebe!U11&gt;1, (src_phoebe!U11-1)*(src_phoebe!T11^2), 0) + IF(src_usha!U11&gt;1, (src_usha!U11-1)*(src_usha!T11^2), 0)) / (V8 - COUNTIF(V8:V8, ""))))</f>
-        <v>0.86615818416730328</v>
+        <v>0.80759628819471574</v>
       </c>
       <c r="V8" s="9">
         <f>IF((src_susan!U11 + src_adam!U11 + src_kenton!U11 + src_phoebe!U11 + src_usha!U11)=0, "", (src_susan!U11 + src_adam!U11 + src_kenton!U11 + src_phoebe!U11 + src_usha!U11))</f>
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="X8" s="27">
         <f>IF(Z8="", "", (src_susan!W11*src_susan!Y11 + src_adam!W11*src_adam!Y11 + src_kenton!W11*src_kenton!Y11 + src_phoebe!W11*src_phoebe!Y11 + src_usha!W11*src_usha!Y11)/Z8)</f>
-        <v>2.507936507936508E-2</v>
+        <v>2.7867647058823528E-2</v>
       </c>
       <c r="Y8" s="27">
         <f>IF(Z8="", "", SQRT((IF(src_susan!Y11&gt;1, (src_susan!Y11-1)*(src_susan!X11^2), 0) + IF(src_adam!Y11&gt;1, (src_adam!Y11-1)*(src_adam!X11^2), 0) + IF(src_kenton!Y11&gt;1, (src_kenton!Y11-1)*(src_kenton!X11^2), 0) + IF(src_phoebe!Y11&gt;1, (src_phoebe!Y11-1)*(src_phoebe!X11^2), 0) + IF(src_usha!Y11&gt;1, (src_usha!Y11-1)*(src_usha!X11^2), 0)) / (Z8 - COUNTIF(Z8:Z8, ""))))</f>
-        <v>0.49336818838689767</v>
+        <v>0.50201432484834652</v>
       </c>
       <c r="Z8" s="9">
         <f>IF((src_susan!Y11 + src_adam!Y11 + src_kenton!Y11 + src_phoebe!Y11 + src_usha!Y11)=0, "", (src_susan!Y11 + src_adam!Y11 + src_kenton!Y11 + src_phoebe!Y11 + src_usha!Y11))</f>
-        <v>189</v>
+        <v>272</v>
       </c>
       <c r="AA8" s="9"/>
       <c r="AB8" s="28">
         <f t="shared" ref="AB8:AB30" si="0">IF(F8="", "", (D8*H8 + H8*J8 + L8*N8 + P8*R8 + T8*V8 + X8*Z8) / (H8 + J8 + N8 + R8 + V8 + Z8))</f>
-        <v>0.42144172856989848</v>
+        <v>0.36683949537962146</v>
       </c>
       <c r="AC8" s="52">
         <f>AB8-AVG_ALL</f>
-        <v>-0.12869534282281903</v>
+        <v>-9.3932263268131311E-2</v>
       </c>
       <c r="AD8" s="28">
         <f t="shared" ref="AD8:AD30" si="1">IF(SUM(F8, J8, N8, R8, V8, Z8)&lt;=1, "", SQRT(
@@ -2082,7 +2165,7 @@
    IF(Z8&gt;1, (Z8-1)*Y8^2, 0)) /
   (SUM(F8, J8, N8, R8, V8, Z8) - 6)
 ))</f>
-        <v>1.3280907755996243</v>
+        <v>1.2465388249628728</v>
       </c>
       <c r="AE8" s="8"/>
       <c r="AF8" s="18" t="s">
@@ -2146,40 +2229,40 @@
       </c>
       <c r="T9" s="27">
         <f>IF(V9="", "", (src_susan!S12*src_susan!U12 + src_adam!S12*src_adam!U12 + src_kenton!S12*src_kenton!U12 + src_phoebe!S12*src_phoebe!U12 + src_usha!S12*src_usha!U12)/V9)</f>
-        <v>0.36355555555555552</v>
+        <v>0.35712418300653598</v>
       </c>
       <c r="U9" s="27">
         <f>IF(V9="", "", SQRT((IF(src_susan!U12&gt;1, (src_susan!U12-1)*(src_susan!T12^2), 0) + IF(src_adam!U12&gt;1, (src_adam!U12-1)*(src_adam!T12^2), 0) + IF(src_kenton!U12&gt;1, (src_kenton!U12-1)*(src_kenton!T12^2), 0) + IF(src_phoebe!U12&gt;1, (src_phoebe!U12-1)*(src_phoebe!T12^2), 0) + IF(src_usha!U12&gt;1, (src_usha!U12-1)*(src_usha!T12^2), 0)) / (V9 - COUNTIF(V9:V9, ""))))</f>
-        <v>1.0508287734503234</v>
+        <v>1.1146927241536322</v>
       </c>
       <c r="V9" s="9">
         <f>IF((src_susan!U12 + src_adam!U12 + src_kenton!U12 + src_phoebe!U12 + src_usha!U12)=0, "", (src_susan!U12 + src_adam!U12 + src_kenton!U12 + src_phoebe!U12 + src_usha!U12))</f>
-        <v>90</v>
+        <v>153</v>
       </c>
       <c r="X9" s="27">
         <f>IF(Z9="", "", (src_susan!W12*src_susan!Y12 + src_adam!W12*src_adam!Y12 + src_kenton!W12*src_kenton!Y12 + src_phoebe!W12*src_phoebe!Y12 + src_usha!W12*src_usha!Y12)/Z9)</f>
-        <v>0.4151595744680851</v>
+        <v>0.35059040590405899</v>
       </c>
       <c r="Y9" s="27">
         <f>IF(Z9="", "", SQRT((IF(src_susan!Y12&gt;1, (src_susan!Y12-1)*(src_susan!X12^2), 0) + IF(src_adam!Y12&gt;1, (src_adam!Y12-1)*(src_adam!X12^2), 0) + IF(src_kenton!Y12&gt;1, (src_kenton!Y12-1)*(src_kenton!X12^2), 0) + IF(src_phoebe!Y12&gt;1, (src_phoebe!Y12-1)*(src_phoebe!X12^2), 0) + IF(src_usha!Y12&gt;1, (src_usha!Y12-1)*(src_usha!X12^2), 0)) / (Z9 - COUNTIF(Z9:Z9, ""))))</f>
-        <v>0.96159165482979203</v>
+        <v>0.86723933204196313</v>
       </c>
       <c r="Z9" s="9">
         <f>IF((src_susan!Y12 + src_adam!Y12 + src_kenton!Y12 + src_phoebe!Y12 + src_usha!Y12)=0, "", (src_susan!Y12 + src_adam!Y12 + src_kenton!Y12 + src_phoebe!Y12 + src_usha!Y12))</f>
-        <v>188</v>
+        <v>271</v>
       </c>
       <c r="AA9" s="9"/>
       <c r="AB9" s="28">
         <f t="shared" si="0"/>
-        <v>0.75061061263786188</v>
+        <v>0.66741306690111002</v>
       </c>
       <c r="AC9" s="52">
         <f>AB9-AVG_ALL</f>
-        <v>0.20047354124514438</v>
+        <v>0.20664130825335725</v>
       </c>
       <c r="AD9" s="28">
         <f t="shared" si="1"/>
-        <v>1.6452384541658744</v>
+        <v>1.5556443620636853</v>
       </c>
       <c r="AE9" s="8"/>
       <c r="AF9" s="18" t="s">
@@ -2243,40 +2326,40 @@
       </c>
       <c r="T10" s="27">
         <f>IF(V10="", "", (src_susan!S13*src_susan!U13 + src_adam!S13*src_adam!U13 + src_kenton!S13*src_kenton!U13 + src_phoebe!S13*src_phoebe!U13 + src_usha!S13*src_usha!U13)/V10)</f>
-        <v>0.31077777777777782</v>
+        <v>0.22646616541353384</v>
       </c>
       <c r="U10" s="27">
         <f>IF(V10="", "", SQRT((IF(src_susan!U13&gt;1, (src_susan!U13-1)*(src_susan!T13^2), 0) + IF(src_adam!U13&gt;1, (src_adam!U13-1)*(src_adam!T13^2), 0) + IF(src_kenton!U13&gt;1, (src_kenton!U13-1)*(src_kenton!T13^2), 0) + IF(src_phoebe!U13&gt;1, (src_phoebe!U13-1)*(src_phoebe!T13^2), 0) + IF(src_usha!U13&gt;1, (src_usha!U13-1)*(src_usha!T13^2), 0)) / (V10 - COUNTIF(V10:V10, ""))))</f>
-        <v>1.2178715495121442</v>
+        <v>1.09579236274745</v>
       </c>
       <c r="V10" s="9">
         <f>IF((src_susan!U13 + src_adam!U13 + src_kenton!U13 + src_phoebe!U13 + src_usha!U13)=0, "", (src_susan!U13 + src_adam!U13 + src_kenton!U13 + src_phoebe!U13 + src_usha!U13))</f>
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="X10" s="27">
         <f>IF(Z10="", "", (src_susan!W13*src_susan!Y13 + src_adam!W13*src_adam!Y13 + src_kenton!W13*src_kenton!Y13 + src_phoebe!W13*src_phoebe!Y13 + src_usha!W13*src_usha!Y13)/Z10)</f>
-        <v>9.8835978835978833E-2</v>
+        <v>0.10850202429149798</v>
       </c>
       <c r="Y10" s="27">
         <f>IF(Z10="", "", SQRT((IF(src_susan!Y13&gt;1, (src_susan!Y13-1)*(src_susan!X13^2), 0) + IF(src_adam!Y13&gt;1, (src_adam!Y13-1)*(src_adam!X13^2), 0) + IF(src_kenton!Y13&gt;1, (src_kenton!Y13-1)*(src_kenton!X13^2), 0) + IF(src_phoebe!Y13&gt;1, (src_phoebe!Y13-1)*(src_phoebe!X13^2), 0) + IF(src_usha!Y13&gt;1, (src_usha!Y13-1)*(src_usha!X13^2), 0)) / (Z10 - COUNTIF(Z10:Z10, ""))))</f>
-        <v>0.81535268442558029</v>
+        <v>0.84415686321713879</v>
       </c>
       <c r="Z10" s="9">
         <f>IF((src_susan!Y13 + src_adam!Y13 + src_kenton!Y13 + src_phoebe!Y13 + src_usha!Y13)=0, "", (src_susan!Y13 + src_adam!Y13 + src_kenton!Y13 + src_phoebe!Y13 + src_usha!Y13))</f>
-        <v>189</v>
+        <v>247</v>
       </c>
       <c r="AA10" s="9"/>
       <c r="AB10" s="28">
         <f t="shared" si="0"/>
-        <v>0.41301453889048145</v>
+        <v>0.37450246124465336</v>
       </c>
       <c r="AC10" s="52">
         <f>AB10-AVG_ALL</f>
-        <v>-0.13712253250223605</v>
+        <v>-8.626929740309941E-2</v>
       </c>
       <c r="AD10" s="28">
         <f t="shared" si="1"/>
-        <v>1.5102129797817465</v>
+        <v>1.4541565069141398</v>
       </c>
       <c r="AE10" s="8"/>
       <c r="AF10" s="18" t="s">
@@ -2340,40 +2423,40 @@
       </c>
       <c r="T11" s="27">
         <f>IF(V11="", "", (src_susan!S14*src_susan!U14 + src_adam!S14*src_adam!U14 + src_kenton!S14*src_kenton!U14 + src_phoebe!S14*src_phoebe!U14 + src_usha!S14*src_usha!U14)/V11)</f>
-        <v>0.26119402985074625</v>
+        <v>0.15884615384615383</v>
       </c>
       <c r="U11" s="27">
         <f>IF(V11="", "", SQRT((IF(src_susan!U14&gt;1, (src_susan!U14-1)*(src_susan!T14^2), 0) + IF(src_adam!U14&gt;1, (src_adam!U14-1)*(src_adam!T14^2), 0) + IF(src_kenton!U14&gt;1, (src_kenton!U14-1)*(src_kenton!T14^2), 0) + IF(src_phoebe!U14&gt;1, (src_phoebe!U14-1)*(src_phoebe!T14^2), 0) + IF(src_usha!U14&gt;1, (src_usha!U14-1)*(src_usha!T14^2), 0)) / (V11 - COUNTIF(V11:V11, ""))))</f>
-        <v>0.86960275713907476</v>
+        <v>0.78323883772644787</v>
       </c>
       <c r="V11" s="9">
         <f>IF((src_susan!U14 + src_adam!U14 + src_kenton!U14 + src_phoebe!U14 + src_usha!U14)=0, "", (src_susan!U14 + src_adam!U14 + src_kenton!U14 + src_phoebe!U14 + src_usha!U14))</f>
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="X11" s="27">
         <f>IF(Z11="", "", (src_susan!W14*src_susan!Y14 + src_adam!W14*src_adam!Y14 + src_kenton!W14*src_kenton!Y14 + src_phoebe!W14*src_phoebe!Y14 + src_usha!W14*src_usha!Y14)/Z11)</f>
-        <v>0.3</v>
+        <v>0.20974619289340099</v>
       </c>
       <c r="Y11" s="27">
         <f>IF(Z11="", "", SQRT((IF(src_susan!Y14&gt;1, (src_susan!Y14-1)*(src_susan!X14^2), 0) + IF(src_adam!Y14&gt;1, (src_adam!Y14-1)*(src_adam!X14^2), 0) + IF(src_kenton!Y14&gt;1, (src_kenton!Y14-1)*(src_kenton!X14^2), 0) + IF(src_phoebe!Y14&gt;1, (src_phoebe!Y14-1)*(src_phoebe!X14^2), 0) + IF(src_usha!Y14&gt;1, (src_usha!Y14-1)*(src_usha!X14^2), 0)) / (Z11 - COUNTIF(Z11:Z11, ""))))</f>
-        <v>0.80371560388599184</v>
+        <v>0.72423073138625094</v>
       </c>
       <c r="Z11" s="9">
         <f>IF((src_susan!Y14 + src_adam!Y14 + src_kenton!Y14 + src_phoebe!Y14 + src_usha!Y14)=0, "", (src_susan!Y14 + src_adam!Y14 + src_kenton!Y14 + src_phoebe!Y14 + src_usha!Y14))</f>
-        <v>114</v>
+        <v>197</v>
       </c>
       <c r="AA11" s="9"/>
       <c r="AB11" s="28">
         <f t="shared" si="0"/>
-        <v>0.50597538917196072</v>
+        <v>0.39585999526617538</v>
       </c>
       <c r="AC11" s="52">
         <f>AB11-AVG_ALL</f>
-        <v>-4.4161682220756782E-2</v>
+        <v>-6.4911763381577392E-2</v>
       </c>
       <c r="AD11" s="28">
         <f t="shared" si="1"/>
-        <v>1.5928041379619278</v>
+        <v>1.4330157876062104</v>
       </c>
       <c r="AE11" s="8"/>
       <c r="AF11" s="18" t="s">
@@ -2435,39 +2518,46 @@
         <f>IF((src_susan!Q15 + src_adam!Q15 + src_kenton!Q15 + src_phoebe!Q15 + src_usha!Q15)=0, "", (src_susan!Q15 + src_adam!Q15 + src_kenton!Q15 + src_phoebe!Q15 + src_usha!Q15))</f>
         <v/>
       </c>
-      <c r="T12" s="27" t="str">
+      <c r="T12" s="27">
         <f>IF(V12="", "", (src_susan!S15*src_susan!U15 + src_adam!S15*src_adam!U15 + src_kenton!S15*src_kenton!U15 + src_phoebe!S15*src_phoebe!U15 + src_usha!S15*src_usha!U15)/V12)</f>
-        <v/>
-      </c>
-      <c r="U12" s="27" t="str">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U12" s="27">
         <f>IF(V12="", "", SQRT((IF(src_susan!U15&gt;1, (src_susan!U15-1)*(src_susan!T15^2), 0) + IF(src_adam!U15&gt;1, (src_adam!U15-1)*(src_adam!T15^2), 0) + IF(src_kenton!U15&gt;1, (src_kenton!U15-1)*(src_kenton!T15^2), 0) + IF(src_phoebe!U15&gt;1, (src_phoebe!U15-1)*(src_phoebe!T15^2), 0) + IF(src_usha!U15&gt;1, (src_usha!U15-1)*(src_usha!T15^2), 0)) / (V12 - COUNTIF(V12:V12, ""))))</f>
-        <v/>
-      </c>
-      <c r="V12" s="9" t="str">
+        <v>0.99818672811555975</v>
+      </c>
+      <c r="V12" s="9">
         <f>IF((src_susan!U15 + src_adam!U15 + src_kenton!U15 + src_phoebe!U15 + src_usha!U15)=0, "", (src_susan!U15 + src_adam!U15 + src_kenton!U15 + src_phoebe!U15 + src_usha!U15))</f>
-        <v/>
-      </c>
-      <c r="X12" s="27" t="str">
+        <v>43</v>
+      </c>
+      <c r="X12" s="27">
         <f>IF(Z12="", "", (src_susan!W15*src_susan!Y15 + src_adam!W15*src_adam!Y15 + src_kenton!W15*src_kenton!Y15 + src_phoebe!W15*src_phoebe!Y15 + src_usha!W15*src_usha!Y15)/Z12)</f>
-        <v/>
-      </c>
-      <c r="Y12" s="27" t="str">
+        <v>0.05</v>
+      </c>
+      <c r="Y12" s="27">
         <f>IF(Z12="", "", SQRT((IF(src_susan!Y15&gt;1, (src_susan!Y15-1)*(src_susan!X15^2), 0) + IF(src_adam!Y15&gt;1, (src_adam!Y15-1)*(src_adam!X15^2), 0) + IF(src_kenton!Y15&gt;1, (src_kenton!Y15-1)*(src_kenton!X15^2), 0) + IF(src_phoebe!Y15&gt;1, (src_phoebe!Y15-1)*(src_phoebe!X15^2), 0) + IF(src_usha!Y15&gt;1, (src_usha!Y15-1)*(src_usha!X15^2), 0)) / (Z12 - COUNTIF(Z12:Z12, ""))))</f>
-        <v/>
-      </c>
-      <c r="Z12" s="9" t="str">
+        <v>0.34696963993191499</v>
+      </c>
+      <c r="Z12" s="9">
         <f>IF((src_susan!Y15 + src_adam!Y15 + src_kenton!Y15 + src_phoebe!Y15 + src_usha!Y15)=0, "", (src_susan!Y15 + src_adam!Y15 + src_kenton!Y15 + src_phoebe!Y15 + src_usha!Y15))</f>
-        <v/>
+        <v>58</v>
       </c>
       <c r="AA12" s="9"/>
-      <c r="AB12" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="AC12" s="52"/>
-      <c r="AD12" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="AB12" s="28">
+        <f>IF(V12="", "", (T12*V12 + X12*Z12) / (V12 + Z12))</f>
+        <v>8.831683168316834E-2</v>
+      </c>
+      <c r="AC12" s="52">
+        <f>AB12-AVG_ALL</f>
+        <v>-0.37245492696458443</v>
+      </c>
+      <c r="AD12" s="28">
+        <f>IF(SUM(V12, Z12)&lt;=1, "", SQRT(
+  (IF(V12&gt;1, (V12-1)*U12^2, 0) +
+   IF(Z12&gt;1, (Z12-1)*Y12^2, 0)) /
+  (SUM(V12, Z12) - 6)
+))</f>
+        <v>0.71605597638276031</v>
       </c>
       <c r="AE12" s="8"/>
       <c r="AF12" s="18" t="s">
@@ -2560,7 +2650,7 @@
       </c>
       <c r="AC13" s="52">
         <f>AB13-AVG_ALL</f>
-        <v>-0.33749408523979757</v>
+        <v>-0.24812877249483284</v>
       </c>
       <c r="AD13" s="28">
         <f t="shared" si="1"/>
@@ -2657,7 +2747,7 @@
       </c>
       <c r="AC14" s="52">
         <f>AB14-AVG_ALL</f>
-        <v>-6.9323117904345366E-2</v>
+        <v>2.0042194840619365E-2</v>
       </c>
       <c r="AD14" s="28">
         <f t="shared" si="1"/>
@@ -2754,7 +2844,7 @@
       </c>
       <c r="AC15" s="52">
         <f>AB15-AVG_ALL</f>
-        <v>4.9044503476982526E-2</v>
+        <v>0.13840981622194726</v>
       </c>
       <c r="AD15" s="28">
         <f t="shared" si="1"/>
@@ -2820,39 +2910,46 @@
         <f>IF((src_susan!Q19 + src_adam!Q19 + src_kenton!Q19 + src_phoebe!Q19 + src_usha!Q19)=0, "", (src_susan!Q19 + src_adam!Q19 + src_kenton!Q19 + src_phoebe!Q19 + src_usha!Q19))</f>
         <v/>
       </c>
-      <c r="T16" s="27" t="str">
+      <c r="T16" s="27">
         <f>IF(V16="", "", (src_susan!S19*src_susan!U19 + src_adam!S19*src_adam!U19 + src_kenton!S19*src_kenton!U19 + src_phoebe!S19*src_phoebe!U19 + src_usha!S19*src_usha!U19)/V16)</f>
-        <v/>
-      </c>
-      <c r="U16" s="27" t="str">
+        <v>0.05</v>
+      </c>
+      <c r="U16" s="27">
         <f>IF(V16="", "", SQRT((IF(src_susan!U19&gt;1, (src_susan!U19-1)*(src_susan!T19^2), 0) + IF(src_adam!U19&gt;1, (src_adam!U19-1)*(src_adam!T19^2), 0) + IF(src_kenton!U19&gt;1, (src_kenton!U19-1)*(src_kenton!T19^2), 0) + IF(src_phoebe!U19&gt;1, (src_phoebe!U19-1)*(src_phoebe!T19^2), 0) + IF(src_usha!U19&gt;1, (src_usha!U19-1)*(src_usha!T19^2), 0)) / (V16 - COUNTIF(V16:V16, ""))))</f>
-        <v/>
-      </c>
-      <c r="V16" s="9" t="str">
+        <v>1.2865768535147832</v>
+      </c>
+      <c r="V16" s="9">
         <f>IF((src_susan!U19 + src_adam!U19 + src_kenton!U19 + src_phoebe!U19 + src_usha!U19)=0, "", (src_susan!U19 + src_adam!U19 + src_kenton!U19 + src_phoebe!U19 + src_usha!U19))</f>
-        <v/>
-      </c>
-      <c r="X16" s="27" t="str">
+        <v>20</v>
+      </c>
+      <c r="X16" s="27">
         <f>IF(Z16="", "", (src_susan!W19*src_susan!Y19 + src_adam!W19*src_adam!Y19 + src_kenton!W19*src_kenton!Y19 + src_phoebe!W19*src_phoebe!Y19 + src_usha!W19*src_usha!Y19)/Z16)</f>
-        <v/>
-      </c>
-      <c r="Y16" s="27" t="str">
+        <v>0.12</v>
+      </c>
+      <c r="Y16" s="27">
         <f>IF(Z16="", "", SQRT((IF(src_susan!Y19&gt;1, (src_susan!Y19-1)*(src_susan!X19^2), 0) + IF(src_adam!Y19&gt;1, (src_adam!Y19-1)*(src_adam!X19^2), 0) + IF(src_kenton!Y19&gt;1, (src_kenton!Y19-1)*(src_kenton!X19^2), 0) + IF(src_phoebe!Y19&gt;1, (src_phoebe!Y19-1)*(src_phoebe!X19^2), 0) + IF(src_usha!Y19&gt;1, (src_usha!Y19-1)*(src_usha!X19^2), 0)) / (Z16 - COUNTIF(Z16:Z16, ""))))</f>
-        <v/>
-      </c>
-      <c r="Z16" s="9" t="str">
+        <v>0.51929182547003372</v>
+      </c>
+      <c r="Z16" s="9">
         <f>IF((src_susan!Y19 + src_adam!Y19 + src_kenton!Y19 + src_phoebe!Y19 + src_usha!Y19)=0, "", (src_susan!Y19 + src_adam!Y19 + src_kenton!Y19 + src_phoebe!Y19 + src_usha!Y19))</f>
-        <v/>
+        <v>25</v>
       </c>
       <c r="AA16" s="9"/>
-      <c r="AB16" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="AC16" s="52"/>
-      <c r="AD16" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="AB16" s="28">
+        <f>IF(V16="", "", (T16*V16 + X16*Z16) / (V16 + Z16))</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="AC16" s="52">
+        <f>AB16-AVG_ALL</f>
+        <v>-0.37188286975886387</v>
+      </c>
+      <c r="AD16" s="28">
+        <f>IF(SUM(V16, Z16)&lt;=1, "", SQRT(
+  (IF(V16&gt;1, (V16-1)*U16^2, 0) +
+   IF(Z16&gt;1, (Z16-1)*Y16^2, 0)) /
+  (SUM(V16, Z16) - 6)
+))</f>
+        <v>0.98608596910286606</v>
       </c>
       <c r="AE16" s="8"/>
       <c r="AF16" s="18" t="s">
@@ -2945,7 +3042,7 @@
       </c>
       <c r="AC17" s="52">
         <f>AB17-AVG_ALL</f>
-        <v>0.55727171898787919</v>
+        <v>0.64663703173284393</v>
       </c>
       <c r="AD17" s="28">
         <f t="shared" si="1"/>
@@ -3042,7 +3139,7 @@
       </c>
       <c r="AC18" s="52">
         <f>AB18-AVG_ALL</f>
-        <v>8.3712982808772152E-2</v>
+        <v>0.17307829555373688</v>
       </c>
       <c r="AD18" s="28">
         <f t="shared" si="1"/>
@@ -3134,12 +3231,12 @@
       </c>
       <c r="AA19" s="9"/>
       <c r="AB19" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(V19="", "", (D19*H19 + H19*J19 + L19*N19 + P19*R19 + T19*V19 + X19*Z19) / (H19 + J19 + N19 + R19 + V19 + Z19))</f>
         <v>0.72255500781531812</v>
       </c>
       <c r="AC19" s="52">
         <f>AB19-AVG_ALL</f>
-        <v>0.17241793642260062</v>
+        <v>0.26178324916756535</v>
       </c>
       <c r="AD19" s="28">
         <f t="shared" si="1"/>
@@ -3205,39 +3302,46 @@
         <f>IF((src_susan!Q23 + src_adam!Q23 + src_kenton!Q23 + src_phoebe!Q23 + src_usha!Q23)=0, "", (src_susan!Q23 + src_adam!Q23 + src_kenton!Q23 + src_phoebe!Q23 + src_usha!Q23))</f>
         <v/>
       </c>
-      <c r="T20" s="27" t="str">
+      <c r="T20" s="27">
         <f>IF(V20="", "", (src_susan!S23*src_susan!U23 + src_adam!S23*src_adam!U23 + src_kenton!S23*src_kenton!U23 + src_phoebe!S23*src_phoebe!U23 + src_usha!S23*src_usha!U23)/V20)</f>
-        <v/>
-      </c>
-      <c r="U20" s="27" t="str">
+        <v>0.05</v>
+      </c>
+      <c r="U20" s="27">
         <f>IF(V20="", "", SQRT((IF(src_susan!U23&gt;1, (src_susan!U23-1)*(src_susan!T23^2), 0) + IF(src_adam!U23&gt;1, (src_adam!U23-1)*(src_adam!T23^2), 0) + IF(src_kenton!U23&gt;1, (src_kenton!U23-1)*(src_kenton!T23^2), 0) + IF(src_phoebe!U23&gt;1, (src_phoebe!U23-1)*(src_phoebe!T23^2), 0) + IF(src_usha!U23&gt;1, (src_usha!U23-1)*(src_usha!T23^2), 0)) / (V20 - COUNTIF(V20:V20, ""))))</f>
-        <v/>
-      </c>
-      <c r="V20" s="9" t="str">
+        <v>0.67252880979181839</v>
+      </c>
+      <c r="V20" s="9">
         <f>IF((src_susan!U23 + src_adam!U23 + src_kenton!U23 + src_phoebe!U23 + src_usha!U23)=0, "", (src_susan!U23 + src_adam!U23 + src_kenton!U23 + src_phoebe!U23 + src_usha!U23))</f>
-        <v/>
-      </c>
-      <c r="X20" s="27" t="str">
+        <v>20</v>
+      </c>
+      <c r="X20" s="27">
         <f>IF(Z20="", "", (src_susan!W23*src_susan!Y23 + src_adam!W23*src_adam!Y23 + src_kenton!W23*src_kenton!Y23 + src_phoebe!W23*src_phoebe!Y23 + src_usha!W23*src_usha!Y23)/Z20)</f>
-        <v/>
-      </c>
-      <c r="Y20" s="27" t="str">
+        <v>-0.04</v>
+      </c>
+      <c r="Y20" s="27">
         <f>IF(Z20="", "", SQRT((IF(src_susan!Y23&gt;1, (src_susan!Y23-1)*(src_susan!X23^2), 0) + IF(src_adam!Y23&gt;1, (src_adam!Y23-1)*(src_adam!X23^2), 0) + IF(src_kenton!Y23&gt;1, (src_kenton!Y23-1)*(src_kenton!X23^2), 0) + IF(src_phoebe!Y23&gt;1, (src_phoebe!Y23-1)*(src_phoebe!X23^2), 0) + IF(src_usha!Y23&gt;1, (src_usha!Y23-1)*(src_usha!X23^2), 0)) / (Z20 - COUNTIF(Z20:Z20, ""))))</f>
-        <v/>
-      </c>
-      <c r="Z20" s="9" t="str">
+        <v>0.44090815370097208</v>
+      </c>
+      <c r="Z20" s="9">
         <f>IF((src_susan!Y23 + src_adam!Y23 + src_kenton!Y23 + src_phoebe!Y23 + src_usha!Y23)=0, "", (src_susan!Y23 + src_adam!Y23 + src_kenton!Y23 + src_phoebe!Y23 + src_usha!Y23))</f>
-        <v/>
+        <v>25</v>
       </c>
       <c r="AA20" s="9"/>
-      <c r="AB20" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="AC20" s="52"/>
-      <c r="AD20" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="AB20" s="28">
+        <f>IF(V20="", "", (T20*V20 + X20*Z20) / (V20 + Z20))</f>
+        <v>0</v>
+      </c>
+      <c r="AC20" s="52">
+        <f>AB20-AVG_ALL</f>
+        <v>-0.46077175864775277</v>
+      </c>
+      <c r="AD20" s="28">
+        <f>IF(SUM(V20, Z20)&lt;=1, "", SQRT(
+  (IF(V20&gt;1, (V20-1)*U20^2, 0) +
+   IF(Z20&gt;1, (Z20-1)*Y20^2, 0)) /
+  (SUM(V20, Z20) - 6)
+))</f>
+        <v>0.58307770955903926</v>
       </c>
       <c r="AE20" s="8"/>
       <c r="AF20" s="18" t="s">
@@ -3299,39 +3403,46 @@
         <f>IF((src_susan!Q24 + src_adam!Q24 + src_kenton!Q24 + src_phoebe!Q24 + src_usha!Q24)=0, "", (src_susan!Q24 + src_adam!Q24 + src_kenton!Q24 + src_phoebe!Q24 + src_usha!Q24))</f>
         <v/>
       </c>
-      <c r="T21" s="27" t="str">
+      <c r="T21" s="27">
         <f>IF(V21="", "", (src_susan!S24*src_susan!U24 + src_adam!S24*src_adam!U24 + src_kenton!S24*src_kenton!U24 + src_phoebe!S24*src_phoebe!U24 + src_usha!S24*src_usha!U24)/V21)</f>
-        <v/>
-      </c>
-      <c r="U21" s="27" t="str">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U21" s="27">
         <f>IF(V21="", "", SQRT((IF(src_susan!U24&gt;1, (src_susan!U24-1)*(src_susan!T24^2), 0) + IF(src_adam!U24&gt;1, (src_adam!U24-1)*(src_adam!T24^2), 0) + IF(src_kenton!U24&gt;1, (src_kenton!U24-1)*(src_kenton!T24^2), 0) + IF(src_phoebe!U24&gt;1, (src_phoebe!U24-1)*(src_phoebe!T24^2), 0) + IF(src_usha!U24&gt;1, (src_usha!U24-1)*(src_usha!T24^2), 0)) / (V21 - COUNTIF(V21:V21, ""))))</f>
-        <v/>
-      </c>
-      <c r="V21" s="9" t="str">
+        <v>0.45461969795362128</v>
+      </c>
+      <c r="V21" s="9">
         <f>IF((src_susan!U24 + src_adam!U24 + src_kenton!U24 + src_phoebe!U24 + src_usha!U24)=0, "", (src_susan!U24 + src_adam!U24 + src_kenton!U24 + src_phoebe!U24 + src_usha!U24))</f>
-        <v/>
-      </c>
-      <c r="X21" s="27" t="str">
+        <v>43</v>
+      </c>
+      <c r="X21" s="27">
         <f>IF(Z21="", "", (src_susan!W24*src_susan!Y24 + src_adam!W24*src_adam!Y24 + src_kenton!W24*src_kenton!Y24 + src_phoebe!W24*src_phoebe!Y24 + src_usha!W24*src_usha!Y24)/Z21)</f>
-        <v/>
-      </c>
-      <c r="Y21" s="27" t="str">
+        <v>-1.9999999999999997E-2</v>
+      </c>
+      <c r="Y21" s="27">
         <f>IF(Z21="", "", SQRT((IF(src_susan!Y24&gt;1, (src_susan!Y24-1)*(src_susan!X24^2), 0) + IF(src_adam!Y24&gt;1, (src_adam!Y24-1)*(src_adam!X24^2), 0) + IF(src_kenton!Y24&gt;1, (src_kenton!Y24-1)*(src_kenton!X24^2), 0) + IF(src_phoebe!Y24&gt;1, (src_phoebe!Y24-1)*(src_phoebe!X24^2), 0) + IF(src_usha!Y24&gt;1, (src_usha!Y24-1)*(src_usha!X24^2), 0)) / (Z21 - COUNTIF(Z21:Z21, ""))))</f>
-        <v/>
-      </c>
-      <c r="Z21" s="9" t="str">
+        <v>0.68402586158006096</v>
+      </c>
+      <c r="Z21" s="9">
         <f>IF((src_susan!Y24 + src_adam!Y24 + src_kenton!Y24 + src_phoebe!Y24 + src_usha!Y24)=0, "", (src_susan!Y24 + src_adam!Y24 + src_kenton!Y24 + src_phoebe!Y24 + src_usha!Y24))</f>
-        <v/>
+        <v>58</v>
       </c>
       <c r="AA21" s="9"/>
-      <c r="AB21" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="AC21" s="52"/>
-      <c r="AD21" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="AB21" s="28">
+        <f t="shared" ref="AB21:AB23" si="2">IF(V21="", "", (T21*V21 + X21*Z21) / (V21 + Z21))</f>
+        <v>1.8316831683168319E-2</v>
+      </c>
+      <c r="AC21" s="52">
+        <f>AB21-AVG_ALL</f>
+        <v>-0.44245492696458444</v>
+      </c>
+      <c r="AD21" s="28">
+        <f>IF(SUM(V21, Z21)&lt;=1, "", SQRT(
+  (IF(V21&gt;1, (V21-1)*U21^2, 0) +
+   IF(Z21&gt;1, (Z21-1)*Y21^2, 0)) /
+  (SUM(V21, Z21) - 6)
+))</f>
+        <v>0.61000715742929656</v>
       </c>
       <c r="AE21" s="8"/>
       <c r="AF21" s="18" t="s">
@@ -3393,39 +3504,46 @@
         <f>IF((src_susan!Q25 + src_adam!Q25 + src_kenton!Q25 + src_phoebe!Q25 + src_usha!Q25)=0, "", (src_susan!Q25 + src_adam!Q25 + src_kenton!Q25 + src_phoebe!Q25 + src_usha!Q25))</f>
         <v/>
       </c>
-      <c r="T22" s="27" t="str">
+      <c r="T22" s="27">
         <f>IF(V22="", "", (src_susan!S25*src_susan!U25 + src_adam!S25*src_adam!U25 + src_kenton!S25*src_kenton!U25 + src_phoebe!S25*src_phoebe!U25 + src_usha!S25*src_usha!U25)/V22)</f>
-        <v/>
-      </c>
-      <c r="U22" s="27" t="str">
+        <v>0.21</v>
+      </c>
+      <c r="U22" s="27">
         <f>IF(V22="", "", SQRT((IF(src_susan!U25&gt;1, (src_susan!U25-1)*(src_susan!T25^2), 0) + IF(src_adam!U25&gt;1, (src_adam!U25-1)*(src_adam!T25^2), 0) + IF(src_kenton!U25&gt;1, (src_kenton!U25-1)*(src_kenton!T25^2), 0) + IF(src_phoebe!U25&gt;1, (src_phoebe!U25-1)*(src_phoebe!T25^2), 0) + IF(src_usha!U25&gt;1, (src_usha!U25-1)*(src_usha!T25^2), 0)) / (V22 - COUNTIF(V22:V22, ""))))</f>
-        <v/>
-      </c>
-      <c r="V22" s="9" t="str">
+        <v>0.66216347310636148</v>
+      </c>
+      <c r="V22" s="9">
         <f>IF((src_susan!U25 + src_adam!U25 + src_kenton!U25 + src_phoebe!U25 + src_usha!U25)=0, "", (src_susan!U25 + src_adam!U25 + src_kenton!U25 + src_phoebe!U25 + src_usha!U25))</f>
-        <v/>
-      </c>
-      <c r="X22" s="27" t="str">
+        <v>43</v>
+      </c>
+      <c r="X22" s="27">
         <f>IF(Z22="", "", (src_susan!W25*src_susan!Y25 + src_adam!W25*src_adam!Y25 + src_kenton!W25*src_kenton!Y25 + src_phoebe!W25*src_phoebe!Y25 + src_usha!W25*src_usha!Y25)/Z22)</f>
-        <v/>
-      </c>
-      <c r="Y22" s="27" t="str">
+        <v>0.12</v>
+      </c>
+      <c r="Y22" s="27">
         <f>IF(Z22="", "", SQRT((IF(src_susan!Y25&gt;1, (src_susan!Y25-1)*(src_susan!X25^2), 0) + IF(src_adam!Y25&gt;1, (src_adam!Y25-1)*(src_adam!X25^2), 0) + IF(src_kenton!Y25&gt;1, (src_kenton!Y25-1)*(src_kenton!X25^2), 0) + IF(src_phoebe!Y25&gt;1, (src_phoebe!Y25-1)*(src_phoebe!X25^2), 0) + IF(src_usha!Y25&gt;1, (src_usha!Y25-1)*(src_usha!X25^2), 0)) / (Z22 - COUNTIF(Z22:Z22, ""))))</f>
-        <v/>
-      </c>
-      <c r="Z22" s="9" t="str">
+        <v>0.37670989478322203</v>
+      </c>
+      <c r="Z22" s="9">
         <f>IF((src_susan!Y25 + src_adam!Y25 + src_kenton!Y25 + src_phoebe!Y25 + src_usha!Y25)=0, "", (src_susan!Y25 + src_adam!Y25 + src_kenton!Y25 + src_phoebe!Y25 + src_usha!Y25))</f>
-        <v/>
+        <v>58</v>
       </c>
       <c r="AA22" s="9"/>
-      <c r="AB22" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="AC22" s="52"/>
-      <c r="AD22" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="AB22" s="28">
+        <f t="shared" si="2"/>
+        <v>0.15831683168316829</v>
+      </c>
+      <c r="AC22" s="52">
+        <f>AB22-AVG_ALL</f>
+        <v>-0.30245492696458448</v>
+      </c>
+      <c r="AD22" s="28">
+        <f>IF(SUM(V22, Z22)&lt;=1, "", SQRT(
+  (IF(V22&gt;1, (V22-1)*U22^2, 0) +
+   IF(Z22&gt;1, (Z22-1)*Y22^2, 0)) /
+  (SUM(V22, Z22) - 6)
+))</f>
+        <v>0.52819682525656775</v>
       </c>
       <c r="AE22" s="8"/>
       <c r="AF22" s="18" t="s">
@@ -3487,39 +3605,46 @@
         <f>IF((src_susan!Q26 + src_adam!Q26 + src_kenton!Q26 + src_phoebe!Q26 + src_usha!Q26)=0, "", (src_susan!Q26 + src_adam!Q26 + src_kenton!Q26 + src_phoebe!Q26 + src_usha!Q26))</f>
         <v/>
       </c>
-      <c r="T23" s="27" t="str">
+      <c r="T23" s="27">
         <f>IF(V23="", "", (src_susan!S26*src_susan!U26 + src_adam!S26*src_adam!U26 + src_kenton!S26*src_kenton!U26 + src_phoebe!S26*src_phoebe!U26 + src_usha!S26*src_usha!U26)/V23)</f>
-        <v/>
-      </c>
-      <c r="U23" s="27" t="str">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="U23" s="27">
         <f>IF(V23="", "", SQRT((IF(src_susan!U26&gt;1, (src_susan!U26-1)*(src_susan!T26^2), 0) + IF(src_adam!U26&gt;1, (src_adam!U26-1)*(src_adam!T26^2), 0) + IF(src_kenton!U26&gt;1, (src_kenton!U26-1)*(src_kenton!T26^2), 0) + IF(src_phoebe!U26&gt;1, (src_phoebe!U26-1)*(src_phoebe!T26^2), 0) + IF(src_usha!U26&gt;1, (src_usha!U26-1)*(src_usha!T26^2), 0)) / (V23 - COUNTIF(V23:V23, ""))))</f>
-        <v/>
-      </c>
-      <c r="V23" s="9" t="str">
+        <v>1.0080697650275952</v>
+      </c>
+      <c r="V23" s="9">
         <f>IF((src_susan!U26 + src_adam!U26 + src_kenton!U26 + src_phoebe!U26 + src_usha!U26)=0, "", (src_susan!U26 + src_adam!U26 + src_kenton!U26 + src_phoebe!U26 + src_usha!U26))</f>
-        <v/>
-      </c>
-      <c r="X23" s="27" t="str">
+        <v>43</v>
+      </c>
+      <c r="X23" s="27">
         <f>IF(Z23="", "", (src_susan!W26*src_susan!Y26 + src_adam!W26*src_adam!Y26 + src_kenton!W26*src_kenton!Y26 + src_phoebe!W26*src_phoebe!Y26 + src_usha!W26*src_usha!Y26)/Z23)</f>
-        <v/>
-      </c>
-      <c r="Y23" s="27" t="str">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Y23" s="27">
         <f>IF(Z23="", "", SQRT((IF(src_susan!Y26&gt;1, (src_susan!Y26-1)*(src_susan!X26^2), 0) + IF(src_adam!Y26&gt;1, (src_adam!Y26-1)*(src_adam!X26^2), 0) + IF(src_kenton!Y26&gt;1, (src_kenton!Y26-1)*(src_kenton!X26^2), 0) + IF(src_phoebe!Y26&gt;1, (src_phoebe!Y26-1)*(src_phoebe!X26^2), 0) + IF(src_usha!Y26&gt;1, (src_usha!Y26-1)*(src_usha!X26^2), 0)) / (Z23 - COUNTIF(Z23:Z23, ""))))</f>
-        <v/>
-      </c>
-      <c r="Z23" s="9" t="str">
+        <v>0.58489167874237102</v>
+      </c>
+      <c r="Z23" s="9">
         <f>IF((src_susan!Y26 + src_adam!Y26 + src_kenton!Y26 + src_phoebe!Y26 + src_usha!Y26)=0, "", (src_susan!Y26 + src_adam!Y26 + src_kenton!Y26 + src_phoebe!Y26 + src_usha!Y26))</f>
-        <v/>
+        <v>58</v>
       </c>
       <c r="AA23" s="9"/>
-      <c r="AB23" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="AC23" s="52"/>
-      <c r="AD23" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="AB23" s="28">
+        <f t="shared" si="2"/>
+        <v>6.1485148514851491E-2</v>
+      </c>
+      <c r="AC23" s="52">
+        <f>AB23-AVG_ALL</f>
+        <v>-0.39928661013290129</v>
+      </c>
+      <c r="AD23" s="28">
+        <f>IF(SUM(V23, Z23)&lt;=1, "", SQRT(
+  (IF(V23&gt;1, (V23-1)*U23^2, 0) +
+   IF(Z23&gt;1, (Z23-1)*Y23^2, 0)) /
+  (SUM(V23, Z23) - 6)
+))</f>
+        <v>0.80902928886526948</v>
       </c>
       <c r="AE23" s="8"/>
       <c r="AF23" s="18" t="s">
@@ -3612,7 +3737,7 @@
       </c>
       <c r="AC24" s="52">
         <f>AB24-AVG_ALL</f>
-        <v>5.3633380965319E-2</v>
+        <v>0.14299869371028373</v>
       </c>
       <c r="AD24" s="28">
         <f t="shared" si="1"/>
@@ -3709,7 +3834,7 @@
       </c>
       <c r="AC25" s="52">
         <f>AB25-AVG_ALL</f>
-        <v>0.16253411555311348</v>
+        <v>0.25189942829807821</v>
       </c>
       <c r="AD25" s="28">
         <f t="shared" si="1"/>
@@ -3806,7 +3931,7 @@
       </c>
       <c r="AC26" s="52">
         <f>AB26-AVG_ALL</f>
-        <v>0.75168926075969378</v>
+        <v>0.84105457350465851</v>
       </c>
       <c r="AD26" s="28">
         <f t="shared" si="1"/>
@@ -3903,7 +4028,7 @@
       </c>
       <c r="AC27" s="52">
         <f>AB27-AVG_ALL</f>
-        <v>0.26712832011953591</v>
+        <v>0.35649363286450064</v>
       </c>
       <c r="AD27" s="28">
         <f t="shared" si="1"/>
@@ -4000,7 +4125,7 @@
       </c>
       <c r="AC28" s="52">
         <f>AB28-AVG_ALL</f>
-        <v>0.42344158328396708</v>
+        <v>0.51280689602893181</v>
       </c>
       <c r="AD28" s="28">
         <f t="shared" si="1"/>
@@ -4032,21 +4157,36 @@
       <c r="P29" s="27"/>
       <c r="Q29" s="20"/>
       <c r="R29" s="9"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="20"/>
-      <c r="V29" s="9"/>
-      <c r="X29" s="27"/>
+      <c r="T29" s="27" t="str">
+        <f>IF(V29="", "", (src_susan!S32*src_susan!U32 + src_adam!S32*src_adam!U32 + src_kenton!S32*src_kenton!U32 + src_phoebe!S32*src_phoebe!U32 + src_usha!S32*src_usha!U32)/V29)</f>
+        <v/>
+      </c>
+      <c r="U29" s="27" t="str">
+        <f>IF(V29="", "", SQRT((IF(src_susan!U32&gt;1, (src_susan!U32-1)*(src_susan!T32^2), 0) + IF(src_adam!U32&gt;1, (src_adam!U32-1)*(src_adam!T32^2), 0) + IF(src_kenton!U32&gt;1, (src_kenton!U32-1)*(src_kenton!T32^2), 0) + IF(src_phoebe!U32&gt;1, (src_phoebe!U32-1)*(src_phoebe!T32^2), 0) + IF(src_usha!U32&gt;1, (src_usha!U32-1)*(src_usha!T32^2), 0)) / (V29 - COUNTIF(V29:V29, ""))))</f>
+        <v/>
+      </c>
+      <c r="V29" s="9" t="str">
+        <f>IF((src_susan!U32 + src_adam!U32 + src_kenton!U32 + src_phoebe!U32 + src_usha!U32)=0, "", (src_susan!U32 + src_adam!U32 + src_kenton!U32 + src_phoebe!U32 + src_usha!U32))</f>
+        <v/>
+      </c>
+      <c r="X29" s="27" t="str">
+        <f>IF(Z29="", "", (src_susan!W32*src_susan!Y32 + src_adam!W32*src_adam!Y32 + src_kenton!W32*src_kenton!Y32 + src_phoebe!W32*src_phoebe!Y32 + src_usha!W32*src_usha!Y32)/Z29)</f>
+        <v/>
+      </c>
       <c r="Y29" s="27" t="str">
         <f>IF(Z29="", "", SQRT((IF(src_susan!Y32&gt;1, (src_susan!Y32-1)*(src_susan!X32^2), 0) + IF(src_adam!Y32&gt;1, (src_adam!Y32-1)*(src_adam!X32^2), 0) + IF(src_kenton!Y32&gt;1, (src_kenton!Y32-1)*(src_kenton!X32^2), 0) + IF(src_phoebe!Y32&gt;1, (src_phoebe!Y32-1)*(src_phoebe!X32^2), 0) + IF(src_usha!Y32&gt;1, (src_usha!Y32-1)*(src_usha!X32^2), 0)) / (Z29 - COUNTIF(Z29:Z29, ""))))</f>
         <v/>
       </c>
-      <c r="Z29" s="9"/>
+      <c r="Z29" s="9" t="str">
+        <f>IF((src_susan!Y32 + src_adam!Y32 + src_kenton!Y32 + src_phoebe!Y32 + src_usha!Y32)=0, "", (src_susan!Y32 + src_adam!Y32 + src_kenton!Y32 + src_phoebe!Y32 + src_usha!Y32))</f>
+        <v/>
+      </c>
       <c r="AA29" s="9"/>
       <c r="AB29" s="28" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AC29" s="28"/>
+      <c r="AC29" s="52"/>
       <c r="AD29" s="28" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -4108,37 +4248,38 @@
       </c>
       <c r="T30" s="28">
         <f>IF(V30="", "", (src_susan!S8*src_susan!U8 + src_adam!S8*src_adam!U8 + src_kenton!S8*src_kenton!U8 + src_phoebe!S8*src_phoebe!U8 + src_usha!S8*src_usha!U8)/V30)</f>
-        <v>9.6631716906946274E-2</v>
+        <v>7.9385826771653553E-2</v>
       </c>
       <c r="U30" s="28">
         <f>IF(V30="", "", SQRT((IF(src_susan!U8&gt;1, (src_susan!U8-1)*(src_susan!T8^2), 0) + IF(src_adam!U8&gt;1, (src_adam!U8-1)*(src_adam!T8^2), 0) + IF(src_kenton!U8&gt;1, (src_kenton!U8-1)*(src_kenton!T8^2), 0) + IF(src_phoebe!U8&gt;1, (src_phoebe!U8-1)*(src_phoebe!T8^2), 0) + IF(src_usha!U8&gt;1, (src_usha!U8-1)*(src_usha!T8^2), 0)) / (V30 - COUNTIF(V30:V30, ""))))</f>
-        <v>1.0027779240068517</v>
+        <v>0.95128466805948231</v>
       </c>
       <c r="V30" s="12">
         <f>IF((src_susan!U8 + src_adam!U8 + src_kenton!U8 + src_phoebe!U8 + src_usha!U8)=0, "", (src_susan!U8 + src_adam!U8 + src_kenton!U8 + src_phoebe!U8 + src_usha!U8))</f>
-        <v>763</v>
-      </c>
+        <v>1270</v>
+      </c>
+      <c r="W30" s="6"/>
       <c r="X30" s="28">
         <f>IF(Z30="", "", (src_susan!W8*src_susan!Y8 + src_adam!W8*src_adam!Y8 + src_kenton!W8*src_kenton!Y8 + src_phoebe!W8*src_phoebe!Y8 + src_usha!W8*src_usha!Y8)/Z30)</f>
-        <v>-5.3794037940379409E-3</v>
+        <v>-8.7523277467411586E-4</v>
       </c>
       <c r="Y30" s="28">
         <f>IF(Z30="", "", SQRT((IF(src_susan!Y8&gt;1, (src_susan!Y8-1)*(src_susan!X8^2), 0) + IF(src_adam!Y8&gt;1, (src_adam!Y8-1)*(src_adam!X8^2), 0) + IF(src_kenton!Y8&gt;1, (src_kenton!Y8-1)*(src_kenton!X8^2), 0) + IF(src_phoebe!Y8&gt;1, (src_phoebe!Y8-1)*(src_phoebe!X8^2), 0) + IF(src_usha!Y8&gt;1, (src_usha!Y8-1)*(src_usha!X8^2), 0)) / (Z30 - COUNTIF(Z30:Z30, ""))))</f>
-        <v>0.77813401636573776</v>
+        <v>0.72316872038121405</v>
       </c>
       <c r="Z30" s="12">
         <f>IF((src_susan!Y8 + src_adam!Y8 + src_kenton!Y8 + src_phoebe!Y8 + src_usha!Y8)=0, "", (src_susan!Y8 + src_adam!Y8 + src_kenton!Y8 + src_phoebe!Y8 + src_usha!Y8))</f>
-        <v>1476</v>
+        <v>2148</v>
       </c>
       <c r="AA30" s="12"/>
       <c r="AB30" s="28">
         <f t="shared" si="0"/>
-        <v>0.5501370713927175</v>
-      </c>
-      <c r="AC30" s="28"/>
+        <v>0.46077175864775277</v>
+      </c>
+      <c r="AC30" s="52"/>
       <c r="AD30" s="28">
         <f t="shared" si="1"/>
-        <v>1.4828238517302645</v>
+        <v>1.3942886935285985</v>
       </c>
       <c r="AE30" s="11"/>
       <c r="AF30" s="17" t="s">
@@ -4250,7 +4391,7 @@
     <mergeCell ref="T4:V4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
@@ -4264,7 +4405,7 @@
   <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8093,10 +8234,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:AA41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8349,12 +8490,24 @@
       <c r="O8" s="27"/>
       <c r="P8" s="20"/>
       <c r="Q8" s="1"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="1"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="1"/>
+      <c r="S8" s="26">
+        <v>0</v>
+      </c>
+      <c r="T8" s="19">
+        <v>0.96</v>
+      </c>
+      <c r="U8" s="1">
+        <v>120</v>
+      </c>
+      <c r="W8" s="26">
+        <v>0.11</v>
+      </c>
+      <c r="X8" s="19">
+        <v>0.49</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>150</v>
+      </c>
       <c r="AA8" s="16" t="s">
         <v>10</v>
       </c>
@@ -8396,12 +8549,24 @@
       <c r="O10" s="27"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="9"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="8"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="2"/>
+      <c r="S10" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="T10" s="19">
+        <v>0.72</v>
+      </c>
+      <c r="U10" s="2">
+        <v>20</v>
+      </c>
+      <c r="W10" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="X10" s="19">
+        <v>0.35</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>25</v>
+      </c>
       <c r="AA10" s="18" t="s">
         <v>40</v>
       </c>
@@ -8422,12 +8587,24 @@
       <c r="O11" s="27"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="9"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="8"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="2"/>
+      <c r="S11" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="T11" s="19">
+        <v>0.99</v>
+      </c>
+      <c r="U11" s="2">
+        <v>20</v>
+      </c>
+      <c r="W11" s="26">
+        <v>0.16</v>
+      </c>
+      <c r="X11" s="19">
+        <v>0.47</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>25</v>
+      </c>
       <c r="AA11" s="18" t="s">
         <v>26</v>
       </c>
@@ -8448,12 +8625,24 @@
       <c r="O12" s="27"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="9"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="8"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="2"/>
+      <c r="S12" s="26">
+        <v>0.15</v>
+      </c>
+      <c r="T12" s="19">
+        <v>0.93</v>
+      </c>
+      <c r="U12" s="2">
+        <v>20</v>
+      </c>
+      <c r="W12" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="X12" s="19">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>25</v>
+      </c>
       <c r="AA12" s="18" t="s">
         <v>27</v>
       </c>
@@ -8500,12 +8689,24 @@
       <c r="O14" s="27"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="9"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="9"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="20"/>
-      <c r="Y14" s="2"/>
+      <c r="S14" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="T14" s="19">
+        <v>1</v>
+      </c>
+      <c r="U14" s="2">
+        <v>20</v>
+      </c>
+      <c r="W14" s="26">
+        <v>-0.04</v>
+      </c>
+      <c r="X14" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>25</v>
+      </c>
       <c r="AA14" s="18" t="s">
         <v>28</v>
       </c>
@@ -8630,12 +8831,24 @@
       <c r="O19" s="27"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="9"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="20"/>
-      <c r="U19" s="9"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="9"/>
+      <c r="S19" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="T19" s="19">
+        <v>1.32</v>
+      </c>
+      <c r="U19" s="9">
+        <v>20</v>
+      </c>
+      <c r="W19" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="X19" s="19">
+        <v>0.53</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>25</v>
+      </c>
       <c r="AA19" s="18" t="s">
         <v>29</v>
       </c>
@@ -8734,12 +8947,24 @@
       <c r="O23" s="27"/>
       <c r="P23" s="20"/>
       <c r="Q23" s="9"/>
-      <c r="S23" s="27"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="9"/>
-      <c r="W23" s="27"/>
-      <c r="X23" s="20"/>
-      <c r="Y23" s="9"/>
+      <c r="S23" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="T23" s="19">
+        <v>0.69</v>
+      </c>
+      <c r="U23" s="2">
+        <v>20</v>
+      </c>
+      <c r="W23" s="26">
+        <v>-0.04</v>
+      </c>
+      <c r="X23" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>25</v>
+      </c>
       <c r="AA23" s="18" t="s">
         <v>32</v>
       </c>
@@ -8952,66 +9177,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:22">
       <c r="A33" s="14"/>
     </row>
-    <row r="34" spans="1:27" s="5" customFormat="1">
-      <c r="A34" s="14"/>
-      <c r="B34"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="2"/>
-      <c r="F34"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="2"/>
-      <c r="J34"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="2"/>
-      <c r="N34"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="2"/>
-      <c r="R34"/>
-      <c r="S34" s="26"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="2"/>
-      <c r="V34"/>
-      <c r="W34" s="26"/>
-      <c r="X34" s="19"/>
-      <c r="Y34" s="2"/>
-      <c r="Z34"/>
-      <c r="AA34" s="16"/>
-    </row>
-    <row r="35" spans="1:27" s="5" customFormat="1">
-      <c r="A35" s="14"/>
-      <c r="B35"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="2"/>
-      <c r="F35"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="2"/>
-      <c r="J35"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="2"/>
-      <c r="N35"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="2"/>
-      <c r="R35"/>
-      <c r="S35" s="26"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="2"/>
-      <c r="V35"/>
-      <c r="W35" s="26"/>
-      <c r="X35" s="19"/>
-      <c r="Y35" s="2"/>
-      <c r="Z35"/>
-      <c r="AA35" s="16"/>
+    <row r="35" spans="1:22">
+      <c r="V35" s="62"/>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="V36" s="62"/>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="V37" s="62"/>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="V38" s="62"/>
+    </row>
+    <row r="39" spans="1:22">
+      <c r="V39" s="62"/>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="V40" s="62"/>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="V41" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -9033,10 +9221,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9289,12 +9477,24 @@
       <c r="O8" s="27"/>
       <c r="P8" s="20"/>
       <c r="Q8" s="1"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="1"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="1"/>
+      <c r="S8" s="26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T8" s="19">
+        <v>0.84</v>
+      </c>
+      <c r="U8" s="2">
+        <v>387</v>
+      </c>
+      <c r="W8" s="26">
+        <v>-0.02</v>
+      </c>
+      <c r="X8" s="19">
+        <v>0.61</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>522</v>
+      </c>
       <c r="AA8" s="16" t="s">
         <v>10</v>
       </c>
@@ -9336,12 +9536,24 @@
       <c r="O10" s="27"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="9"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="8"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="2"/>
+      <c r="S10" s="26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T10" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="U10" s="2">
+        <v>43</v>
+      </c>
+      <c r="W10" s="26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X10" s="19">
+        <v>0.53</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>58</v>
+      </c>
       <c r="AA10" s="18" t="s">
         <v>40</v>
       </c>
@@ -9362,12 +9574,24 @@
       <c r="O11" s="27"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="9"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="8"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="2"/>
+      <c r="S11" s="26">
+        <v>0.09</v>
+      </c>
+      <c r="T11" s="19">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="U11" s="2">
+        <v>43</v>
+      </c>
+      <c r="W11" s="26">
+        <v>-0.02</v>
+      </c>
+      <c r="X11" s="19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>58</v>
+      </c>
       <c r="AA11" s="18" t="s">
         <v>26</v>
       </c>
@@ -9388,12 +9612,24 @@
       <c r="O12" s="27"/>
       <c r="P12" s="20"/>
       <c r="Q12" s="9"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="8"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="2"/>
+      <c r="S12" s="26">
+        <v>0.44</v>
+      </c>
+      <c r="T12" s="19">
+        <v>1.33</v>
+      </c>
+      <c r="U12" s="2">
+        <v>43</v>
+      </c>
+      <c r="W12" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="X12" s="19">
+        <v>0.62</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>58</v>
+      </c>
       <c r="AA12" s="18" t="s">
         <v>27</v>
       </c>
@@ -9414,12 +9650,24 @@
       <c r="O13" s="27"/>
       <c r="P13" s="20"/>
       <c r="Q13" s="9"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="8"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="2"/>
+      <c r="S13" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="T13" s="19">
+        <v>0.79</v>
+      </c>
+      <c r="U13" s="2">
+        <v>43</v>
+      </c>
+      <c r="W13" s="26">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="X13" s="19">
+        <v>0.94</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>58</v>
+      </c>
       <c r="AA13" s="18" t="s">
         <v>41</v>
       </c>
@@ -9440,12 +9688,24 @@
       <c r="O14" s="27"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="9"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="9"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="20"/>
-      <c r="Y14" s="2"/>
+      <c r="S14" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="T14" s="19">
+        <v>0.49</v>
+      </c>
+      <c r="U14" s="2">
+        <v>43</v>
+      </c>
+      <c r="W14" s="26">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="X14" s="19">
+        <v>0.66</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>58</v>
+      </c>
       <c r="AA14" s="18" t="s">
         <v>28</v>
       </c>
@@ -9466,12 +9726,24 @@
       <c r="O15" s="27"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="9"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="9"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="9"/>
+      <c r="S15" s="26">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T15" s="19">
+        <v>1.01</v>
+      </c>
+      <c r="U15" s="2">
+        <v>43</v>
+      </c>
+      <c r="W15" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="X15" s="19">
+        <v>0.35</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>58</v>
+      </c>
       <c r="AA15" s="18" t="s">
         <v>48</v>
       </c>
@@ -9700,12 +9972,24 @@
       <c r="O24" s="27"/>
       <c r="P24" s="20"/>
       <c r="Q24" s="9"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="9"/>
-      <c r="W24" s="27"/>
-      <c r="X24" s="20"/>
-      <c r="Y24" s="9"/>
+      <c r="S24" s="26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T24" s="19">
+        <v>0.46</v>
+      </c>
+      <c r="U24" s="2">
+        <v>43</v>
+      </c>
+      <c r="W24" s="26">
+        <v>-0.02</v>
+      </c>
+      <c r="X24" s="19">
+        <v>0.69</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>58</v>
+      </c>
       <c r="AA24" s="18" t="s">
         <v>45</v>
       </c>
@@ -9726,12 +10010,24 @@
       <c r="O25" s="27"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="9"/>
-      <c r="S25" s="27"/>
-      <c r="T25" s="20"/>
-      <c r="U25" s="9"/>
-      <c r="W25" s="27"/>
-      <c r="X25" s="20"/>
-      <c r="Y25" s="9"/>
+      <c r="S25" s="26">
+        <v>0.21</v>
+      </c>
+      <c r="T25" s="19">
+        <v>0.67</v>
+      </c>
+      <c r="U25" s="2">
+        <v>43</v>
+      </c>
+      <c r="W25" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="X25" s="19">
+        <v>0.38</v>
+      </c>
+      <c r="Y25" s="2">
+        <v>58</v>
+      </c>
       <c r="AA25" s="18" t="s">
         <v>33</v>
       </c>
@@ -9752,12 +10048,24 @@
       <c r="O26" s="27"/>
       <c r="P26" s="20"/>
       <c r="Q26" s="9"/>
-      <c r="S26" s="27"/>
-      <c r="T26" s="20"/>
-      <c r="U26" s="9"/>
-      <c r="W26" s="27"/>
-      <c r="X26" s="20"/>
-      <c r="Y26" s="9"/>
+      <c r="S26" s="26">
+        <v>0.05</v>
+      </c>
+      <c r="T26" s="19">
+        <v>1.02</v>
+      </c>
+      <c r="U26" s="2">
+        <v>43</v>
+      </c>
+      <c r="W26" s="26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X26" s="19">
+        <v>0.59</v>
+      </c>
+      <c r="Y26" s="2">
+        <v>58</v>
+      </c>
       <c r="AA26" s="18" t="s">
         <v>34</v>
       </c>
@@ -9778,12 +10086,6 @@
       <c r="O27" s="27"/>
       <c r="P27" s="20"/>
       <c r="Q27" s="9"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="20"/>
-      <c r="U27" s="9"/>
-      <c r="W27" s="27"/>
-      <c r="X27" s="20"/>
-      <c r="Y27" s="9"/>
       <c r="AA27" s="18" t="s">
         <v>35</v>
       </c>
@@ -9892,67 +10194,6 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
-      <c r="A33" s="14"/>
-    </row>
-    <row r="34" spans="1:27" s="5" customFormat="1">
-      <c r="A34" s="14"/>
-      <c r="B34"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="2"/>
-      <c r="F34"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="2"/>
-      <c r="J34"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="2"/>
-      <c r="N34"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="2"/>
-      <c r="R34"/>
-      <c r="S34" s="26"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="2"/>
-      <c r="V34"/>
-      <c r="W34" s="26"/>
-      <c r="X34" s="19"/>
-      <c r="Y34" s="2"/>
-      <c r="Z34"/>
-      <c r="AA34" s="16"/>
-    </row>
-    <row r="35" spans="1:27" s="5" customFormat="1">
-      <c r="A35" s="14"/>
-      <c r="B35"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="2"/>
-      <c r="F35"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="2"/>
-      <c r="J35"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="2"/>
-      <c r="N35"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="2"/>
-      <c r="R35"/>
-      <c r="S35" s="26"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="2"/>
-      <c r="V35"/>
-      <c r="W35" s="26"/>
-      <c r="X35" s="19"/>
-      <c r="Y35" s="2"/>
-      <c r="Z35"/>
-      <c r="AA35" s="16"/>
-    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="C4:Y4"/>

</xml_diff>